<commit_message>
Refactoring, updates, bug fixes, SQL optimizations
</commit_message>
<xml_diff>
--- a/pkg/excels/report/Balance Report.xlsx
+++ b/pkg/excels/report/Balance Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115F0865-05AE-445C-B2FA-B7B59F064ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D234DFF6-087E-40BF-837C-8E4196017A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Наименование</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Код</t>
+  </si>
+  <si>
+    <t>Сумма</t>
+  </si>
+  <si>
+    <t>Из них негодно</t>
   </si>
 </sst>
 </file>
@@ -357,20 +363,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
     <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -384,7 +394,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>